<commit_message>
adding last  escenarios normalized
</commit_message>
<xml_diff>
--- a/data/NephropsFU30_indices-2.xlsx
+++ b/data/NephropsFU30_indices-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauriciomardones/IEO/Nephrops_SA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBF15CE-8286-E84A-BE52-27021F449E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB87512-CF64-444B-8233-8F7776B41393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -3644,8 +3644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3731,10 +3731,6 @@
         <f>F2/$F$35</f>
         <v>0.7798736861150839</v>
       </c>
-      <c r="I2">
-        <f>G2/$G$35</f>
-        <v>0.79448689923341709</v>
-      </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -3803,10 +3799,6 @@
         <f t="shared" ref="H5:H33" si="0">F5/$F$35</f>
         <v>0.46285323174805287</v>
       </c>
-      <c r="I5">
-        <f t="shared" ref="I5:I33" si="1">G5/$G$35</f>
-        <v>0.93845566112900791</v>
-      </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -3838,10 +3830,6 @@
         <f t="shared" si="0"/>
         <v>0.28983614514321432</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>1.1413822908126523</v>
-      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -3873,10 +3861,6 @@
         <f t="shared" si="0"/>
         <v>0.15148350643332195</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>1.0490586253275997</v>
-      </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -3899,10 +3883,6 @@
         <f t="shared" si="0"/>
         <v>0.46278552139089374</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>1.0890912334910541</v>
-      </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -3934,10 +3914,6 @@
         <f t="shared" si="0"/>
         <v>0.43030169985724348</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>0.8514907384250785</v>
-      </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -3969,10 +3945,6 @@
         <f t="shared" si="0"/>
         <v>0.48075381122602528</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>0.81509570341431481</v>
-      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -4003,10 +3975,6 @@
       <c r="H11" s="4">
         <f t="shared" si="0"/>
         <v>0.67091782690977264</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0.98460213449696299</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -4040,7 +4008,7 @@
         <v>1.7849745969848718</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" ref="E13:E18" si="2">B13/$B$35</f>
+        <f t="shared" ref="E13:E18" si="1">B13/$B$35</f>
         <v>0.14000257358412976</v>
       </c>
       <c r="F13" s="4">
@@ -4052,10 +4020,6 @@
       <c r="H13" s="4">
         <f t="shared" si="0"/>
         <v>0.31257802633384596</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>1.1381654006147028</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -4075,7 +4039,7 @@
         <v>7.618100892023393</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.58541357993181864</v>
       </c>
       <c r="F14" s="4">
@@ -4087,10 +4051,6 @@
       <c r="H14" s="4">
         <f t="shared" si="0"/>
         <v>0.74378396260968549</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>0.98398999745830484</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -4110,7 +4070,7 @@
         <v>3.17983767478299</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.38523204008737361</v>
       </c>
       <c r="F15" s="4">
@@ -4122,10 +4082,6 @@
       <c r="H15" s="4">
         <f t="shared" si="0"/>
         <v>0.53966573795408002</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>0.8885339684023974</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -4145,7 +4101,7 @@
         <v>4.7148857802802846</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.33053004600739022</v>
       </c>
       <c r="F16" s="4">
@@ -4157,10 +4113,6 @@
       <c r="H16" s="4">
         <f t="shared" si="0"/>
         <v>0.4733009704944674</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>0.8630267632549351</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -4180,7 +4132,7 @@
         <v>7.4105549423664776</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.78523272651525056</v>
       </c>
       <c r="F17" s="4">
@@ -4192,10 +4144,6 @@
       <c r="H17" s="4">
         <f t="shared" si="0"/>
         <v>0.85237991006273905</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>0.88252376415060096</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -4215,7 +4163,7 @@
         <v>5.6129021183829249</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.44016510838124007</v>
       </c>
       <c r="F18" s="4">
@@ -4227,10 +4175,6 @@
       <c r="H18" s="4">
         <f t="shared" si="0"/>
         <v>0.33721620521187035</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>1.0435310470592285</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -4254,10 +4198,6 @@
         <f t="shared" si="0"/>
         <v>1.0786173211505006</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
-        <v>1.1511345419071779</v>
-      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -4276,7 +4216,7 @@
         <v>2.373807606018381</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" ref="E20:E29" si="3">B20/$B$35</f>
+        <f t="shared" ref="E20:E29" si="2">B20/$B$35</f>
         <v>0.21774153198488505</v>
       </c>
       <c r="F20" s="4">
@@ -4288,10 +4228,6 @@
       <c r="H20" s="4">
         <f t="shared" si="0"/>
         <v>0.46998032976157433</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>1.1842075383413053</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -4311,7 +4247,7 @@
         <v>2.8332857618441785</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.16746162916585566</v>
       </c>
       <c r="F21" s="4">
@@ -4323,10 +4259,6 @@
       <c r="H21" s="4">
         <f t="shared" si="0"/>
         <v>0.25649174853975515</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
-        <v>1.3004164146879729</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -4346,7 +4278,7 @@
         <v>14.622372864539217</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.73375853317909334</v>
       </c>
       <c r="F22" s="4">
@@ -4358,10 +4290,6 @@
       <c r="H22" s="4">
         <f t="shared" si="0"/>
         <v>0.36481173498970826</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
-        <v>1.0193968313664423</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -4381,7 +4309,7 @@
         <v>29.24696288292127</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.7744624945870646</v>
       </c>
       <c r="F23" s="4">
@@ -4393,10 +4321,6 @@
       <c r="H23" s="4">
         <f t="shared" si="0"/>
         <v>1.2084348991153477</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
-        <v>1.0159161534618402</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -4416,7 +4340,7 @@
         <v>13.232150759711734</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.1717423075984772</v>
       </c>
       <c r="F24" s="4">
@@ -4428,10 +4352,6 @@
       <c r="H24" s="4">
         <f t="shared" si="0"/>
         <v>1.7672852849602669</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="1"/>
-        <v>0.95564708175563162</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -4451,7 +4371,7 @@
         <v>29.072149016723593</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.5246127350281573</v>
       </c>
       <c r="F25" s="4">
@@ -4463,10 +4383,6 @@
       <c r="H25" s="4">
         <f t="shared" si="0"/>
         <v>3.1413183459476914</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="1"/>
-        <v>0.98311063705062729</v>
       </c>
       <c r="J25">
         <v>2327.7983450000002</v>
@@ -4497,7 +4413,7 @@
         <v>25.778811778790512</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.5424135041285096</v>
       </c>
       <c r="F26" s="4">
@@ -4510,10 +4426,6 @@
         <f t="shared" si="0"/>
         <v>1.4951162223057592</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="1"/>
-        <v>1.1421457894858755</v>
-      </c>
       <c r="J26">
         <v>1806.2367320000001</v>
       </c>
@@ -4525,7 +4437,7 @@
         <v>0.86611476147655764</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26:M34" si="4">K26/$K$35</f>
+        <f t="shared" ref="M26:M34" si="3">K26/$K$35</f>
         <v>1.3603385731559856</v>
       </c>
     </row>
@@ -4543,7 +4455,7 @@
         <v>3.4909818299902007</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.35236512776832807</v>
       </c>
       <c r="F27" s="4">
@@ -4556,10 +4468,6 @@
         <f t="shared" si="0"/>
         <v>0.47559770857078071</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="1"/>
-        <v>0.79135752023626538</v>
-      </c>
       <c r="J27">
         <v>2354.6344389999999</v>
       </c>
@@ -4571,7 +4479,7 @@
         <v>1.1290788241477159</v>
       </c>
       <c r="M27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.0882708585247884</v>
       </c>
     </row>
@@ -4589,7 +4497,7 @@
         <v>17.260389686105821</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.2397181878624268</v>
       </c>
       <c r="F28" s="4">
@@ -4602,10 +4510,6 @@
         <f t="shared" si="0"/>
         <v>2.0268815887950993</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="1"/>
-        <v>1.0653750739392804</v>
-      </c>
       <c r="J28">
         <v>3567.0277970000002</v>
       </c>
@@ -4617,7 +4521,7 @@
         <v>1.7104377155247144</v>
       </c>
       <c r="M28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.0229746070133012</v>
       </c>
     </row>
@@ -4635,7 +4539,7 @@
         <v>62.85303906403945</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6883710992819827</v>
       </c>
       <c r="F29" s="4">
@@ -4647,10 +4551,6 @@
       <c r="H29" s="4">
         <f t="shared" si="0"/>
         <v>5.4609633317910777</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="1"/>
-        <v>0.87248659806743156</v>
       </c>
       <c r="L29" s="2"/>
     </row>
@@ -4675,7 +4575,7 @@
         <v>1.2472901452289988</v>
       </c>
       <c r="M30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.0900846432889963</v>
       </c>
     </row>
@@ -4706,10 +4606,6 @@
         <f t="shared" si="0"/>
         <v>0.25962781279585456</v>
       </c>
-      <c r="I31">
-        <f t="shared" si="1"/>
-        <v>1.3394774361998054</v>
-      </c>
       <c r="J31">
         <v>1627.815914</v>
       </c>
@@ -4721,7 +4617,7 @@
         <v>0.78055958397033343</v>
       </c>
       <c r="M31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.98307134220072556</v>
       </c>
     </row>
@@ -4752,10 +4648,6 @@
         <f t="shared" si="0"/>
         <v>0.60705664044049901</v>
       </c>
-      <c r="I32">
-        <f t="shared" si="1"/>
-        <v>0.8795902956822701</v>
-      </c>
       <c r="J32">
         <v>1591.8727289999999</v>
       </c>
@@ -4767,7 +4659,7 @@
         <v>0.76332434423046136</v>
       </c>
       <c r="M32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.7255139056831923</v>
       </c>
     </row>
@@ -4798,10 +4690,7 @@
         <f t="shared" si="0"/>
         <v>2.4000867893457838</v>
       </c>
-      <c r="I33" s="13">
-        <f t="shared" si="1"/>
-        <v>0.8363038605478138</v>
-      </c>
+      <c r="I33" s="13"/>
       <c r="J33">
         <v>1778.0281170000001</v>
       </c>
@@ -4813,7 +4702,7 @@
         <v>0.85258835188723636</v>
       </c>
       <c r="M33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.55320435308343407</v>
       </c>
     </row>
@@ -4838,7 +4727,7 @@
         <v>0.53439571673017805</v>
       </c>
       <c r="M34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.99758162031438946</v>
       </c>
     </row>

</xml_diff>